<commit_message>
subir bases de datos
</commit_message>
<xml_diff>
--- a/FUENTES DE DATOS/DATOS/Tijuana-June-2018.xlsx
+++ b/FUENTES DE DATOS/DATOS/Tijuana-June-2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10523"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvelazquez\Google Drive\TIJUANA INDUSTRIAL SECTOR\INFORME TRIMESTRAL\INFORME_TRIMESTRAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergio-mireles/Dropbox (Datoz)/Datoz/Reportes de Mercado Mensuales/2018/6.Junio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32F80A39-A004-498E-B899-BC3D4BB912A1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61766FD9-1DC3-AF49-950D-CE2D6A258807}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estadísticas Generales" sheetId="1" r:id="rId1"/>
@@ -1779,24 +1779,24 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="4" width="20.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" style="5" customWidth="1"/>
-    <col min="6" max="9" width="20.7109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="4" width="20.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="5" customWidth="1"/>
+    <col min="6" max="9" width="20.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="15" t="s">
         <v>1</v>
@@ -1812,7 +1812,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>0.39829192964156673</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>0.47174588065887207</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0.43017892202825314</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>0.40209364826578298</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>0.39854853031304743</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -2141,12 +2141,12 @@
         <v>0.42014315181792039</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="15" t="s">
         <v>1</v>
@@ -2162,7 +2162,7 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>0.47308161332202281</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>0.43444227096178745</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0.39750004626333063</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>0.44064220183486241</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
@@ -2491,12 +2491,12 @@
         <v>0.42927768873033395</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="15" t="s">
         <v>1</v>
@@ -2512,7 +2512,7 @@
       <c r="I28" s="15"/>
       <c r="J28" s="15"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -2608,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>0.40831802309765702</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>20</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>9</v>
       </c>
@@ -2841,12 +2841,12 @@
         <v>0.39943934103255235</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="15" t="s">
         <v>1</v>
@@ -2862,7 +2862,7 @@
       <c r="I41" s="15"/>
       <c r="J41" s="15"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>0.39274665543803217</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>17</v>
       </c>
@@ -3054,7 +3054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>19</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>20</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>9</v>
       </c>
@@ -3191,12 +3191,12 @@
         <v>0.41637332771901608</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="2"/>
       <c r="B54" s="15" t="s">
         <v>1</v>
@@ -3212,7 +3212,7 @@
       <c r="I54" s="15"/>
       <c r="J54" s="15"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>14</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>15</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>16</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>18</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>9</v>
       </c>
@@ -3543,6 +3543,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="I15:J15"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="D54:H54"/>
     <mergeCell ref="I54:J54"/>
@@ -3552,12 +3558,6 @@
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="D41:H41"/>
     <mergeCell ref="I41:J41"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="I15:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="5">
@@ -3578,20 +3578,20 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="5" customWidth="1"/>
-    <col min="4" max="7" width="20.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="5" customWidth="1"/>
+    <col min="4" max="7" width="20.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>191044</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>550565</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>117196</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>110234</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3729,7 +3729,7 @@
         <v>579305</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3752,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -3827,12 +3827,12 @@
         <v>1548344</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>43298</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>550565</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3947,7 +3947,7 @@
         <v>61000</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>187055</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -4068,12 +4068,12 @@
         <v>841918</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -4096,7 +4096,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>147746</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>117196</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>49234</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>330841</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -4257,7 +4257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>9</v>
       </c>
@@ -4309,12 +4309,12 @@
         <v>645017</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -4337,7 +4337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -4429,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>61409</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>9</v>
       </c>
@@ -4550,12 +4550,12 @@
         <v>61409</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -4670,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>9</v>
       </c>
@@ -4808,23 +4808,23 @@
   <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" style="5" customWidth="1"/>
-    <col min="4" max="7" width="20.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" style="5" customWidth="1"/>
+    <col min="4" max="7" width="20.6640625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4870,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>264005</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>63903</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -5060,12 +5060,12 @@
         <v>327908</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -5088,7 +5088,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>264005</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -5301,12 +5301,12 @@
         <v>264005</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>63903</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>
@@ -5467,7 +5467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>9</v>
       </c>
@@ -5542,12 +5542,12 @@
         <v>63903</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -5570,7 +5570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>15</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>16</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -5754,7 +5754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>9</v>
       </c>
@@ -5783,12 +5783,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>14</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -5903,7 +5903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>17</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>18</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>19</v>
       </c>
@@ -5972,7 +5972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -5995,7 +5995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>9</v>
       </c>
@@ -6041,32 +6041,31 @@
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="5" customWidth="1"/>
-    <col min="7" max="8" width="30.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="5" customWidth="1"/>
-    <col min="10" max="11" width="30.7109375" style="5" customWidth="1"/>
-    <col min="12" max="14" width="20.7109375" style="5" customWidth="1"/>
-    <col min="15" max="15" width="25.7109375" style="5" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" style="5" customWidth="1"/>
-    <col min="17" max="17" width="30.7109375" customWidth="1"/>
+    <col min="1" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" style="5" customWidth="1"/>
+    <col min="7" max="8" width="30.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="5" customWidth="1"/>
+    <col min="10" max="11" width="30.6640625" style="5" customWidth="1"/>
+    <col min="12" max="14" width="20.6640625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" style="5" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -6119,7 +6118,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -6169,7 +6168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -6219,7 +6218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -6269,7 +6268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -6319,7 +6318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -6369,7 +6368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -6419,7 +6418,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -6469,7 +6468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -6519,7 +6518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>75</v>
       </c>
@@ -6569,7 +6568,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -6619,7 +6618,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -6669,7 +6668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -6719,7 +6718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>87</v>
       </c>
@@ -6769,7 +6768,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -6819,7 +6818,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>93</v>
       </c>
@@ -6869,7 +6868,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -6922,7 +6921,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -6972,7 +6971,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -7022,7 +7021,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -7072,7 +7071,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>102</v>
       </c>
@@ -7122,7 +7121,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -7172,7 +7171,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -7222,7 +7221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -7272,7 +7271,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -7322,7 +7321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -7372,7 +7371,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>110</v>
       </c>
@@ -7422,7 +7421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>111</v>
       </c>
@@ -7472,7 +7471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>112</v>
       </c>
@@ -7525,7 +7524,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>113</v>
       </c>
@@ -7575,7 +7574,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -7625,7 +7624,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>116</v>
       </c>
@@ -7678,7 +7677,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>117</v>
       </c>
@@ -7731,7 +7730,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>118</v>
       </c>
@@ -7784,7 +7783,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -7834,22 +7833,22 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="20" width="30.7109375" style="5" customWidth="1"/>
-    <col min="21" max="21" width="30.7109375" customWidth="1"/>
+    <col min="1" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="20" width="30.6640625" style="5" customWidth="1"/>
+    <col min="21" max="21" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -7914,7 +7913,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>43101</v>
       </c>
@@ -7976,7 +7975,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43101</v>
       </c>
@@ -8038,7 +8037,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>43102</v>
       </c>
@@ -8100,7 +8099,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>43132</v>
       </c>
@@ -8162,7 +8161,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>43132</v>
       </c>
@@ -8224,7 +8223,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>43132</v>
       </c>
@@ -8286,7 +8285,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>43132</v>
       </c>
@@ -8348,7 +8347,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>43132</v>
       </c>
@@ -8410,7 +8409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>43132</v>
       </c>
@@ -8472,7 +8471,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>43160</v>
       </c>
@@ -8534,7 +8533,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>43160</v>
       </c>
@@ -8596,7 +8595,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>43160</v>
       </c>
@@ -8658,7 +8657,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>43160</v>
       </c>
@@ -8720,7 +8719,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>43160</v>
       </c>
@@ -8782,7 +8781,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>43160</v>
       </c>
@@ -8844,7 +8843,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>43160</v>
       </c>
@@ -8906,7 +8905,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>43221</v>
       </c>
@@ -8968,7 +8967,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>43252</v>
       </c>
@@ -9033,7 +9032,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>43252</v>
       </c>
@@ -9095,7 +9094,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>43252</v>
       </c>
@@ -9157,7 +9156,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>

</xml_diff>